<commit_message>
Removed "PersonStateIdentification" from consolidation, expungement and identifier update
</commit_message>
<xml_diff>
--- a/shared/ojb-resources-common/src/main/resources/ssp/Criminal_History_Update_Reporting/artifacts/service_model/information_model/IEPD/documentation/Criminal_History_Consolidation_Report.xlsx
+++ b/shared/ojb-resources-common/src/main/resources/ssp/Criminal_History_Update_Reporting/artifacts/service_model/information_model/IEPD/documentation/Criminal_History_Consolidation_Report.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26519"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2440" windowWidth="26920" windowHeight="10360"/>
+    <workbookView xWindow="12000" yWindow="1120" windowWidth="26920" windowHeight="10360"/>
   </bookViews>
   <sheets>
     <sheet name="Request" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
   <si>
     <t>Business</t>
   </si>
@@ -36,12 +36,6 @@
     <t>Pre Consolidation Identifiers</t>
   </si>
   <si>
-    <t>Person State Identification ID</t>
-  </si>
-  <si>
-    <t>An identification of a person based on a state-issued ID.</t>
-  </si>
-  <si>
     <t>A number issued by the FBI's Automated Fingerprint Identification System (AFIS) based on submitted fingerprints.</t>
   </si>
   <si>
@@ -60,25 +54,22 @@
     <t>Criminal History Consolidation Report</t>
   </si>
   <si>
-    <t>/CHcr-doc:CriminalHistoryConsolidationReport/nc:Person/CHcr-ext:PreConsolidationIdentifiers/nc:PersonStateIdentification/nc:IdentificationID</t>
-  </si>
-  <si>
-    <t>/CHcr-doc:CriminalHistoryConsolidationReport/nc:Person/CHcr-ext:PreConsolidationIdentifiers/j:PersonFBIIdentification/nc:IdentificationID</t>
-  </si>
-  <si>
-    <t>/CHcr-doc:CriminalHistoryConsolidationReport/nc:Person/CHcr-ext:PostConsolidationIdentifiers/nc:PersonStateIdentification/nc:IdentificationID</t>
-  </si>
-  <si>
-    <t>/CHcr-doc:CriminalHistoryConsolidationReport/nc:Person/CHcr-ext:PostConsolidationIdentifiers/j:PersonFBIIdentification/nc:IdentificationID</t>
-  </si>
-  <si>
     <t>Person State Fingerprint ID</t>
   </si>
   <si>
     <t>An identification of a person based on a Fingerprint ID.</t>
   </si>
   <si>
-    <t>/CHcr-doc:CriminalHistoryConsolidationReport/nc:Person/CHcr-ext:PostConsolidationIdentifiers/j:PersonStateFingerprintIdentification/nc:IdentificationID</t>
+    <t>chc-report-doc:CriminalHistoryConsolidationReport/nc:Person/chc-report-ext:PreConsolidationIdentifiers/j:PersonStateFingerprintIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>chc-report-doc:CriminalHistoryConsolidationReport/nc:Person/chc-report-ext:PreConsolidationIdentifiers/j:PersonFBIIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>chc-report-doc:CriminalHistoryConsolidationReport/nc:Person/chc-report-ext:PostConsolidationIdentifiers/j:PersonStateFingerprintIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>chc-report-doc:CriminalHistoryConsolidationReport/nc:Person/chc-report-ext:PostConsolidationIdentifiers/j:PersonFBIIdentification/nc:IdentificationID</t>
   </si>
 </sst>
 </file>
@@ -644,7 +635,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="44">
+  <cellStyleXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -689,6 +680,10 @@
     <xf numFmtId="0" fontId="19" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -732,7 +727,7 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="44">
+  <cellStyles count="48">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -762,12 +757,16 @@
     <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
     <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
     <cellStyle name="Followed Hyperlink" xfId="43" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="45" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="47" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
     <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
     <cellStyle name="Hyperlink" xfId="42" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="44" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="46" builtinId="8" hidden="1"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
@@ -1075,13 +1074,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B15" sqref="B15"/>
+      <selection pane="bottomRight" activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1102,7 +1101,7 @@
     </row>
     <row r="2" spans="1:3" ht="45" customHeight="1">
       <c r="A2" s="12" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B2" s="13"/>
       <c r="C2" s="5"/>
@@ -1123,16 +1122,16 @@
         <v>4</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C4" s="3"/>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="8" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C5" s="8" t="s">
         <v>13</v>
@@ -1140,10 +1139,10 @@
     </row>
     <row r="6" spans="1:3" ht="28">
       <c r="A6" s="8" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C6" s="8" t="s">
         <v>14</v>
@@ -1151,43 +1150,32 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C7" s="7"/>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="8" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C8" s="8" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" ht="28">
       <c r="A9" s="8" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="28">
-      <c r="A10" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="C10" s="8" t="s">
         <v>16</v>
       </c>
     </row>

</xml_diff>